<commit_message>
removed gps from va refusals
</commit_message>
<xml_diff>
--- a/forms/varefusals/varefusals.xlsx
+++ b/forms/varefusals/varefusals.xlsx
@@ -9,17 +9,17 @@
     <sheet state="visible" name="warnings" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_5DE9E846_3713_4B6A_9280_F19D93A89EBA_.wvu.FilterData">survey!$A$1:$A$29</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FFAB8A60_D78A_4936_8B3A_C89EBC2E6F6E_.wvu.FilterData">survey!$A$1:$A$27</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{5DE9E846-3713-4B6A-9280-F19D93A89EBA}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{FFAB8A60-D78A-4936-8B3A-C89EBC2E6F6E}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="137">
   <si>
     <t>type</t>
   </si>
@@ -292,42 +292,6 @@
   </si>
   <si>
     <t>selected(${reason_no_participate}, 'other')</t>
-  </si>
-  <si>
-    <t>note_geocode</t>
-  </si>
-  <si>
-    <t>### Geocoding</t>
-  </si>
-  <si>
-    <t>### Ukusanyaji wa vipimo vya GPS</t>
-  </si>
-  <si>
-    <t>### Coordenadas Geograficas</t>
-  </si>
-  <si>
-    <t>geopoint</t>
-  </si>
-  <si>
-    <t>hh_geo_location</t>
-  </si>
-  <si>
-    <t>Stand just outside the front door of the house and geocode the location.</t>
-  </si>
-  <si>
-    <t>Simama mbele tu ya mlango wa kuingia kwenye nyumba na ukusanye vipimo vya GPS vya eneo hilo</t>
-  </si>
-  <si>
-    <t>Wait until accuracy is below 6m or 60 seconds, whichever comes first.</t>
-  </si>
-  <si>
-    <t>Subiri hadi accuracy itakapokuwa chini ya mita 6 au baada ya sekunde 60, chochote kitakacho kuja kwanza.</t>
-  </si>
-  <si>
-    <t>Pare fora da porta principal da casa e tire as coordenadas geograficas do local.</t>
-  </si>
-  <si>
-    <t>Espere ate a precisao estar abaixo de 6m or 60 segundos, oque ocorrer primeiro</t>
   </si>
   <si>
     <t>list_name</t>
@@ -515,6 +479,7 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -533,15 +498,15 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Ubuntu Mono"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -549,7 +514,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,12 +565,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
@@ -631,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -707,28 +666,10 @@
     <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -761,10 +702,10 @@
     <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -776,17 +717,17 @@
     <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
@@ -2049,168 +1990,139 @@
     </row>
     <row r="18">
       <c r="A18" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="28"/>
-      <c r="AH18" s="28"/>
-      <c r="AI18" s="28"/>
-      <c r="AJ18" s="28"/>
-      <c r="AK18" s="28"/>
-      <c r="AL18" s="28"/>
-      <c r="AM18" s="28"/>
-      <c r="AN18" s="28"/>
-      <c r="AO18" s="28"/>
-      <c r="AP18" s="28"/>
-      <c r="AQ18" s="28"/>
+        <v>67</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="26"/>
+      <c r="AD18" s="26"/>
+      <c r="AE18" s="26"/>
+      <c r="AF18" s="26"/>
+      <c r="AG18" s="26"/>
+      <c r="AH18" s="26"/>
+      <c r="AI18" s="26"/>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="26"/>
+      <c r="AM18" s="26"/>
+      <c r="AN18" s="26"/>
+      <c r="AO18" s="26"/>
+      <c r="AP18" s="26"/>
+      <c r="AQ18" s="26"/>
     </row>
     <row r="19">
-      <c r="A19" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="28"/>
-      <c r="AG19" s="28"/>
-      <c r="AH19" s="28"/>
-      <c r="AI19" s="28"/>
-      <c r="AJ19" s="28"/>
-      <c r="AK19" s="28"/>
-      <c r="AL19" s="28"/>
-      <c r="AM19" s="28"/>
-      <c r="AN19" s="28"/>
-      <c r="AO19" s="28"/>
-      <c r="AP19" s="28"/>
-      <c r="AQ19" s="28"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
+      <c r="AN19" s="9"/>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="9"/>
+      <c r="AQ19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="G20" s="28"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="28"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
-      <c r="AG20" s="28"/>
-      <c r="AH20" s="28"/>
-      <c r="AI20" s="28"/>
-      <c r="AJ20" s="28"/>
-      <c r="AK20" s="28"/>
-      <c r="AL20" s="28"/>
-      <c r="AM20" s="28"/>
-      <c r="AN20" s="28"/>
-      <c r="AO20" s="28"/>
-      <c r="AP20" s="28"/>
-      <c r="AQ20" s="28"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="9"/>
+      <c r="AO20" s="9"/>
+      <c r="AP20" s="9"/>
+      <c r="AQ20" s="9"/>
     </row>
     <row r="21">
       <c r="A21" s="9"/>
@@ -2219,7 +2131,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="34"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -2261,9 +2173,9 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="G22" s="34"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -2308,7 +2220,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="34"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -2350,9 +2262,10 @@
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="34"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -2397,7 +2310,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="34"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -2436,189 +2349,99 @@
       <c r="AQ25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AQ26" s="9"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="29"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="29"/>
+      <c r="AI26" s="29"/>
+      <c r="AJ26" s="29"/>
+      <c r="AK26" s="29"/>
+      <c r="AL26" s="29"/>
+      <c r="AM26" s="29"/>
+      <c r="AN26" s="29"/>
+      <c r="AO26" s="29"/>
+      <c r="AP26" s="29"/>
+      <c r="AQ26" s="29"/>
     </row>
     <row r="27">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="9"/>
-      <c r="AK27" s="9"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-      <c r="AQ27" s="9"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
-      <c r="X28" s="35"/>
-      <c r="Y28" s="35"/>
-      <c r="Z28" s="35"/>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="35"/>
-      <c r="AC28" s="35"/>
-      <c r="AD28" s="35"/>
-      <c r="AE28" s="35"/>
-      <c r="AF28" s="35"/>
-      <c r="AG28" s="35"/>
-      <c r="AH28" s="35"/>
-      <c r="AI28" s="35"/>
-      <c r="AJ28" s="35"/>
-      <c r="AK28" s="35"/>
-      <c r="AL28" s="35"/>
-      <c r="AM28" s="35"/>
-      <c r="AN28" s="35"/>
-      <c r="AO28" s="35"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="35"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="35"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="35"/>
-      <c r="Z29" s="35"/>
-      <c r="AA29" s="35"/>
-      <c r="AB29" s="35"/>
-      <c r="AC29" s="35"/>
-      <c r="AD29" s="35"/>
-      <c r="AE29" s="35"/>
-      <c r="AF29" s="35"/>
-      <c r="AG29" s="35"/>
-      <c r="AH29" s="35"/>
-      <c r="AI29" s="35"/>
-      <c r="AJ29" s="35"/>
-      <c r="AK29" s="35"/>
-      <c r="AL29" s="35"/>
-      <c r="AM29" s="35"/>
-      <c r="AN29" s="35"/>
-      <c r="AO29" s="35"/>
-      <c r="AP29" s="35"/>
-      <c r="AQ29" s="35"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="29"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" s="29"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{5DE9E846-3713-4B6A-9280-F19D93A89EBA}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$A$29"/>
+    <customSheetView guid="{FFAB8A60-D78A-4936-8B3A-C89EBC2E6F6E}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$A$27"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="A1:A17">
@@ -2646,12 +2469,12 @@
       <formula>"End group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C29">
+  <conditionalFormatting sqref="C18:C27">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>C18&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A29">
+  <conditionalFormatting sqref="A1:A27">
     <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="or_other">
       <formula>NOT(ISERROR(SEARCH(("or_other"),(A1))))</formula>
     </cfRule>
@@ -2677,220 +2500,220 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="36" t="s">
+      <c r="F1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="43"/>
+      <c r="B2" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="43"/>
+      <c r="B3" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="43"/>
+      <c r="B4" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="37"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="43"/>
+      <c r="B5" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="37"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="43"/>
+      <c r="B6" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="37"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="43"/>
+      <c r="A7" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="37"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="43"/>
+      <c r="A8" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:E8">
@@ -2910,47 +2733,47 @@
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>143</v>
+      <c r="A1" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="49" t="s">
+      <c r="A2" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="52">
-        <v>2.02102071E9</v>
+      <c r="E2" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="46">
+        <v>2.021021101E9</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="53"/>
+      <c r="B8" s="47"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -3945,8 +3768,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="48" t="s">
-        <v>148</v>
+      <c r="A1" s="42" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>